<commit_message>
Competition results are now on GitHub
</commit_message>
<xml_diff>
--- a/data/MA/MA_3B_summary.tools.xlsx
+++ b/data/MA/MA_3B_summary.tools.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmoge\Box Sync\Mycoplasma\Experiments\data\MA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmoge\GitHub\MinimalCell\data\MA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E23F5E-EBF2-43AB-AFFF-68504B507097}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D713CD-3E58-40ED-BD1C-90BF0D630592}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="870" yWindow="3210" windowWidth="22410" windowHeight="12930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MA_3B_summary" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1194,8 +1194,8 @@
   <dimension ref="A1:AW62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC1" sqref="AC1"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10179,6 +10179,10 @@
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
+      <c r="I60">
+        <f>_xlfn.STDEV.S(I2:I58)/SQRT(COUNT(I2:I58))</f>
+        <v>1.5620509560630669E-9</v>
+      </c>
       <c r="N60">
         <f>N59/(SUM($N59:$S59))</f>
         <v>1.3435700575815739E-2</v>
@@ -10233,9 +10237,13 @@
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
+      <c r="I61">
+        <f>2*I60</f>
+        <v>3.1241019121261338E-9</v>
+      </c>
       <c r="J61">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>3.1189381073127024E-9</v>
       </c>
       <c r="K61">
         <f>K59/SUM($K59:$S59)</f>

</xml_diff>

<commit_message>
Revert "Competition results are now on GitHub"
This reverts commit 216a627fa0e255337801ff3b9c0fb15ed8c7b66d.
</commit_message>
<xml_diff>
--- a/data/MA/MA_3B_summary.tools.xlsx
+++ b/data/MA/MA_3B_summary.tools.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmoge\GitHub\MinimalCell\data\MA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmoge\Box Sync\Mycoplasma\Experiments\data\MA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D713CD-3E58-40ED-BD1C-90BF0D630592}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E23F5E-EBF2-43AB-AFFF-68504B507097}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="870" yWindow="3210" windowWidth="22410" windowHeight="12930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MA_3B_summary" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1194,8 +1194,8 @@
   <dimension ref="A1:AW62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I62" sqref="I62"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10179,10 +10179,6 @@
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="I60">
-        <f>_xlfn.STDEV.S(I2:I58)/SQRT(COUNT(I2:I58))</f>
-        <v>1.5620509560630669E-9</v>
-      </c>
       <c r="N60">
         <f>N59/(SUM($N59:$S59))</f>
         <v>1.3435700575815739E-2</v>
@@ -10237,13 +10233,9 @@
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="I61">
-        <f>2*I60</f>
-        <v>3.1241019121261338E-9</v>
-      </c>
       <c r="J61">
         <f t="shared" si="28"/>
-        <v>3.1189381073127024E-9</v>
+        <v>0</v>
       </c>
       <c r="K61">
         <f>K59/SUM($K59:$S59)</f>

</xml_diff>

<commit_message>
I updated figures to use Non-minimal label and display +- 1 SEM error bars; volume analysis; unicode arrows...
</commit_message>
<xml_diff>
--- a/data/MA/MA_3B_summary.tools.xlsx
+++ b/data/MA/MA_3B_summary.tools.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmoge\Box Sync\Mycoplasma\Experiments\data\MA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmoge\GitHub\MinimalCell\data\MA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E23F5E-EBF2-43AB-AFFF-68504B507097}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F618BC8-8ABF-4B7A-BA35-E33DF783CFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MA_3B_summary" sheetId="1" r:id="rId1"/>
@@ -1193,9 +1193,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC1" sqref="AC1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10179,6 +10179,10 @@
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
+      <c r="I60">
+        <f>_xlfn.STDEV.S(I2:I58)/SQRT(COUNT(I2:I58))</f>
+        <v>1.5620509560630669E-9</v>
+      </c>
       <c r="N60">
         <f>N59/(SUM($N59:$S59))</f>
         <v>1.3435700575815739E-2</v>

</xml_diff>